<commit_message>
Actualización de archivos de planeación
</commit_message>
<xml_diff>
--- a/Planeacion PetClinic/Plan de pruebas.xlsx
+++ b/Planeacion PetClinic/Plan de pruebas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\pesd_\Escritorio\Plantilla Agile documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\pesd_\Documents\UP-Chiapas\8 Cuatrimestre\Mantenimiento\1  Corte\Planeacion PetClinic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4F0F13-1E8B-44CC-8542-9D76EB050695}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26918BD5-A24E-4383-AA95-ABE335AD4049}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t>Nombre del proyecto</t>
   </si>
@@ -164,6 +164,12 @@
   </si>
   <si>
     <t>No modificar esta parte</t>
+  </si>
+  <si>
+    <t>Comprobar consistencia de diseño del sistema</t>
+  </si>
+  <si>
+    <t>El sistema presenta una consistencia de diseño en todo el sistema, hay un mismo desarrollo de GUI, botones, tablas, formularios, etc.</t>
   </si>
 </sst>
 </file>
@@ -358,6 +364,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -373,7 +380,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -2084,8 +2090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2239,17 +2245,17 @@
       <c r="A7" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="15"/>
+      <c r="C7" s="16"/>
       <c r="D7" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="16"/>
+      <c r="F7" s="17"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -2270,17 +2276,17 @@
       <c r="A8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="16">
         <v>1</v>
       </c>
-      <c r="C8" s="15"/>
+      <c r="C8" s="16"/>
       <c r="D8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="E8" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="18"/>
+      <c r="F8" s="19"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -2301,17 +2307,17 @@
       <c r="A9" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="15"/>
+      <c r="C9" s="16"/>
       <c r="D9" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="19"/>
+      <c r="F9" s="20"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -2332,17 +2338,17 @@
       <c r="A10" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="15"/>
+      <c r="C10" s="16"/>
       <c r="D10" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="16"/>
+      <c r="F10" s="17"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -2747,12 +2753,22 @@
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
     </row>
-    <row r="23" spans="1:21" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
+    <row r="23" spans="1:21" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A23" s="12">
+        <v>11</v>
+      </c>
+      <c r="B23" s="13">
+        <v>43485</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>26</v>
+      </c>
       <c r="F23" s="12"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -4216,7 +4232,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A13:F13 B14:B22 E14:E22</xm:sqref>
+          <xm:sqref>A13:F13 E14:E22 B14:B23</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="22" id="{1C4D6E8F-045C-5F4C-B1D8-7ABA82174623}">
@@ -4378,7 +4394,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A23:F23</xm:sqref>
+          <xm:sqref>A23 C23:F23</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="13" id="{9737A92A-FEF4-CA4F-B314-425F576BBD4E}">
@@ -4634,7 +4650,7 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="15" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización del plan de pruebas
</commit_message>
<xml_diff>
--- a/Planeacion PetClinic/Plan de pruebas.xlsx
+++ b/Planeacion PetClinic/Plan de pruebas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21126"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\pesd_\Documents\UP-Chiapas\8 Cuatrimestre\Mantenimiento\1  Corte\Planeacion PetClinic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\pesd_\Documents\GitHub\Planeacion-PetClinic\Planeacion PetClinic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26918BD5-A24E-4383-AA95-ABE335AD4049}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4270EF3-FAE1-408F-BA71-A86C0B1CEEB0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -94,19 +94,10 @@
     <t>Chorme</t>
   </si>
   <si>
-    <t>Build ofica</t>
-  </si>
-  <si>
-    <t>71.0.3578.98 (build oficial) (64 bits)</t>
-  </si>
-  <si>
     <t>Conjunto de pruebas para su correcta verificación de las funcionalidaes del sistema.</t>
   </si>
   <si>
     <t>Universidad Politécnica de Chiapas, Suchiapa, Chis.</t>
-  </si>
-  <si>
-    <t>XXX</t>
   </si>
   <si>
     <t>Administración de usuarios</t>
@@ -170,6 +161,15 @@
   </si>
   <si>
     <t>El sistema presenta una consistencia de diseño en todo el sistema, hay un mismo desarrollo de GUI, botones, tablas, formularios, etc.</t>
+  </si>
+  <si>
+    <t>Todo bien.</t>
+  </si>
+  <si>
+    <t>Build oficial:</t>
+  </si>
+  <si>
+    <t>72.0.3626.81 (Build oficial) (64 bits)</t>
   </si>
 </sst>
 </file>
@@ -332,7 +332,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -379,6 +379,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -697,15 +700,15 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Apoyo!$A$11" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="Apoyo!$A$11" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Apoyo!$A$20" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="Apoyo!$A$20" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp11.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Apoyo!$A$21" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="Apoyo!$A$21" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
@@ -725,35 +728,35 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Apoyo!$A$12" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="Apoyo!$A$12" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Apoyo!$A$13" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="Apoyo!$A$13" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Apoyo!$A$14" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="Apoyo!$A$14" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Apoyo!$A$15" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="Apoyo!$A$15" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Apoyo!$A$16" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="Apoyo!$A$16" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Apoyo!$A$17" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="Apoyo!$A$17" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp8.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Apoyo!$A$18" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="Apoyo!$A$18" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp9.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Apoyo!$A$19" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="Apoyo!$A$19" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -770,8 +773,8 @@
         <xdr:to>
           <xdr:col>5</xdr:col>
           <xdr:colOff>1036320</xdr:colOff>
-          <xdr:row>13</xdr:row>
-          <xdr:rowOff>121920</xdr:rowOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>396240</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2090,8 +2093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2281,10 +2284,10 @@
       </c>
       <c r="C8" s="16"/>
       <c r="D8" s="11" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="F8" s="19"/>
       <c r="G8" s="1"/>
@@ -2315,7 +2318,7 @@
         <v>4</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F9" s="20"/>
       <c r="G9" s="1"/>
@@ -2346,7 +2349,7 @@
         <v>5</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F10" s="17"/>
       <c r="G10" s="1"/>
@@ -2423,7 +2426,7 @@
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
     </row>
-    <row r="13" spans="1:21" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>1</v>
       </c>
@@ -2436,8 +2439,8 @@
       <c r="D13" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="14" t="s">
-        <v>26</v>
+      <c r="E13" s="21" t="s">
+        <v>45</v>
       </c>
       <c r="F13" s="12"/>
       <c r="G13" s="1"/>
@@ -2464,13 +2467,13 @@
         <v>43485</v>
       </c>
       <c r="C14" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>26</v>
+      <c r="E14" s="21" t="s">
+        <v>45</v>
       </c>
       <c r="F14" s="12"/>
       <c r="G14" s="1"/>
@@ -2497,13 +2500,13 @@
         <v>43485</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>26</v>
+        <v>28</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>45</v>
       </c>
       <c r="F15" s="12"/>
       <c r="G15" s="1"/>
@@ -2530,13 +2533,13 @@
         <v>43485</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>45</v>
       </c>
       <c r="F16" s="12"/>
       <c r="G16" s="1"/>
@@ -2563,13 +2566,13 @@
         <v>43485</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>26</v>
+        <v>31</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>45</v>
       </c>
       <c r="F17" s="12"/>
       <c r="G17" s="1"/>
@@ -2596,13 +2599,13 @@
         <v>43485</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>26</v>
+        <v>33</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>45</v>
       </c>
       <c r="F18" s="12"/>
       <c r="G18" s="1"/>
@@ -2629,13 +2632,13 @@
         <v>43485</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>26</v>
+        <v>39</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>45</v>
       </c>
       <c r="F19" s="12"/>
       <c r="G19" s="1"/>
@@ -2662,13 +2665,13 @@
         <v>43485</v>
       </c>
       <c r="C20" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>26</v>
+      <c r="E20" s="21" t="s">
+        <v>45</v>
       </c>
       <c r="F20" s="12"/>
       <c r="G20" s="1"/>
@@ -2695,13 +2698,13 @@
         <v>43485</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>26</v>
+        <v>37</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>45</v>
       </c>
       <c r="F21" s="12"/>
       <c r="G21" s="1"/>
@@ -2728,13 +2731,13 @@
         <v>43485</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>26</v>
+        <v>41</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>45</v>
       </c>
       <c r="F22" s="12"/>
       <c r="G22" s="1"/>
@@ -2761,13 +2764,13 @@
         <v>43485</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>26</v>
+        <v>44</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>45</v>
       </c>
       <c r="F23" s="12"/>
       <c r="G23" s="1"/>
@@ -3876,8 +3879,8 @@
                   <to>
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>1036320</xdr:colOff>
-                    <xdr:row>13</xdr:row>
-                    <xdr:rowOff>121920</xdr:rowOff>
+                    <xdr:row>12</xdr:row>
+                    <xdr:rowOff>320040</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4232,7 +4235,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A13:F13 E14:E22 B14:B23</xm:sqref>
+          <xm:sqref>A13:F13 B14:B23 E14:E23</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="22" id="{1C4D6E8F-045C-5F4C-B1D8-7ABA82174623}">
@@ -4394,7 +4397,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A23 C23:F23</xm:sqref>
+          <xm:sqref>A23 C23:D23 F23</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="13" id="{9737A92A-FEF4-CA4F-B314-425F576BBD4E}">
@@ -4651,62 +4654,62 @@
   <sheetData>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>